<commit_message>
modified:   DAC.py 	modified:   I2C_ADC_DAC.py 	gui_plot.py 	new_test_sin_dac.py 	sine_wave.py 	test.py 	zero_output.py
</commit_message>
<xml_diff>
--- a/VoltageValues.xlsx
+++ b/VoltageValues.xlsx
@@ -361,47 +361,47 @@
     </row>
     <row r="3" spans="1:1">
       <c r="A3">
-        <v>0.3440104983672598</v>
+        <v>0.336010254219184</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4">
-        <v>0.3440104983672598</v>
+        <v>0.336010254219184</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5">
-        <v>0.3440104983672598</v>
+        <v>0.3380103152562029</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6">
-        <v>0.3440104983672598</v>
+        <v>0.336010254219184</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7">
-        <v>0.3440104983672598</v>
+        <v>0.336010254219184</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8">
-        <v>0.3440104983672598</v>
+        <v>0.336010254219184</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9">
-        <v>0.3440104983672598</v>
+        <v>0.336010254219184</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10">
-        <v>0.3440104983672598</v>
+        <v>0.336010254219184</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11">
-        <v>0.3440104983672598</v>
+        <v>0.336010254219184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>